<commit_message>
Added learning and comments, optimized player using results
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="500" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Gen1" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,14 @@
     <sheet name="Wins2" sheetId="5" r:id="rId4"/>
     <sheet name="Gen3" sheetId="6" r:id="rId5"/>
     <sheet name="Wins3" sheetId="7" r:id="rId6"/>
+    <sheet name="Gen 4" sheetId="8" r:id="rId7"/>
+    <sheet name="Wins 4" sheetId="9" r:id="rId8"/>
+    <sheet name="Gen 5" sheetId="10" r:id="rId9"/>
+    <sheet name="Wins 5" sheetId="11" r:id="rId10"/>
   </sheets>
   <definedNames>
+    <definedName name="results" localSheetId="6">'Gen 4'!$A$1:$F$74</definedName>
+    <definedName name="results" localSheetId="8">'Gen 5'!$A$1:$F$69</definedName>
     <definedName name="results" localSheetId="0">'Gen1'!$A$2:$S$514</definedName>
     <definedName name="results" localSheetId="2">'Gen2'!$A$1:$S$100</definedName>
     <definedName name="results" localSheetId="4">'Gen3'!$A$1:$S$100</definedName>
@@ -113,11 +119,35 @@
       </textFields>
     </textPr>
   </connection>
+  <connection id="4" name="results3" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" codePage="10000" sourceFile="/Users/Rowan/USC/Junior Year/Australia/Classes/COMP30024/results.txt" tab="0" space="1" consecutive="1">
+      <textFields count="6">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="5" name="results4" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" codePage="10000" sourceFile="/Users/Rowan/USC/Junior Year/Australia/Classes/COMP30024/results.txt" tab="0" space="1" consecutive="1">
+      <textFields count="6">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="922" uniqueCount="35">
   <si>
     <t>B</t>
   </si>
@@ -188,6 +218,9 @@
     <t>1,1</t>
   </si>
   <si>
+    <t>2,0</t>
+  </si>
+  <si>
     <t>1,3</t>
   </si>
   <si>
@@ -207,6 +240,18 @@
   </si>
   <si>
     <t>15,3</t>
+  </si>
+  <si>
+    <t>1,0,1</t>
+  </si>
+  <si>
+    <t>2,2</t>
+  </si>
+  <si>
+    <t>4,3,1</t>
+  </si>
+  <si>
+    <t>2,1,1</t>
   </si>
 </sst>
 </file>
@@ -268,6 +313,14 @@
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="results" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="results" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="results" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -535,7 +588,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S514"/>
   <sheetViews>
-    <sheetView topLeftCell="A498" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A391" sqref="A391:I514"/>
     </sheetView>
   </sheetViews>
@@ -30879,11 +30932,490 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>0.99041999999999997</v>
+      </c>
+      <c r="B1">
+        <v>0.34425</v>
+      </c>
+      <c r="C1">
+        <v>0.74646999999999997</v>
+      </c>
+      <c r="D1">
+        <v>4.6640000000000001E-2</v>
+      </c>
+      <c r="E1">
+        <v>0.71260000000000001</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0.61282000000000003</v>
+      </c>
+      <c r="B2">
+        <v>0.32585999999999998</v>
+      </c>
+      <c r="C2">
+        <v>5.1189999999999999E-2</v>
+      </c>
+      <c r="D2">
+        <v>0.70777000000000001</v>
+      </c>
+      <c r="E2">
+        <v>0.74356999999999995</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>0.35022999999999999</v>
+      </c>
+      <c r="B3">
+        <v>0.15390000000000001</v>
+      </c>
+      <c r="C3">
+        <v>0.18507999999999999</v>
+      </c>
+      <c r="D3">
+        <v>0.43325999999999998</v>
+      </c>
+      <c r="E3">
+        <v>0.93557000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>0.53010999999999997</v>
+      </c>
+      <c r="B4">
+        <v>0.23518</v>
+      </c>
+      <c r="C4">
+        <v>0.45567000000000002</v>
+      </c>
+      <c r="D4">
+        <v>0.36456</v>
+      </c>
+      <c r="E4">
+        <v>0.25274999999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>0.90078999999999998</v>
+      </c>
+      <c r="B5">
+        <v>6.1690000000000002E-2</v>
+      </c>
+      <c r="C5">
+        <v>0.16364999999999999</v>
+      </c>
+      <c r="D5">
+        <v>0.14494000000000001</v>
+      </c>
+      <c r="E5">
+        <v>0.70272999999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>6.9940000000000002E-2</v>
+      </c>
+      <c r="B6">
+        <v>3.0290000000000001E-2</v>
+      </c>
+      <c r="C6">
+        <v>0.10782</v>
+      </c>
+      <c r="D6">
+        <v>0.14846000000000001</v>
+      </c>
+      <c r="E6">
+        <v>2.7060000000000001E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>0.79744000000000004</v>
+      </c>
+      <c r="B7">
+        <v>0.93918999999999997</v>
+      </c>
+      <c r="C7">
+        <v>0.24818000000000001</v>
+      </c>
+      <c r="D7">
+        <v>0.20507</v>
+      </c>
+      <c r="E7">
+        <v>0.83004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>0.71872000000000003</v>
+      </c>
+      <c r="B8">
+        <v>1.9279999999999999E-2</v>
+      </c>
+      <c r="C8">
+        <v>0.30670999999999998</v>
+      </c>
+      <c r="D8">
+        <v>8.5629999999999998E-2</v>
+      </c>
+      <c r="E8">
+        <v>0.15526999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>0.59328000000000003</v>
+      </c>
+      <c r="B9">
+        <v>0.18095</v>
+      </c>
+      <c r="C9">
+        <v>0.40860999999999997</v>
+      </c>
+      <c r="D9">
+        <v>0.57730000000000004</v>
+      </c>
+      <c r="E9">
+        <v>0.48866999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>0.26308999999999999</v>
+      </c>
+      <c r="B10">
+        <v>0.35261999999999999</v>
+      </c>
+      <c r="C10">
+        <v>0.83752000000000004</v>
+      </c>
+      <c r="D10">
+        <v>0.81969999999999998</v>
+      </c>
+      <c r="E10">
+        <v>0.95169999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>0.64576999999999996</v>
+      </c>
+      <c r="B11">
+        <v>0.56266000000000005</v>
+      </c>
+      <c r="C11">
+        <v>0.24948999999999999</v>
+      </c>
+      <c r="D11">
+        <v>0.67759000000000003</v>
+      </c>
+      <c r="E11">
+        <v>0.63100999999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>0.70430000000000004</v>
+      </c>
+      <c r="B12">
+        <v>0.68369000000000002</v>
+      </c>
+      <c r="C12">
+        <v>0.25791999999999998</v>
+      </c>
+      <c r="D12">
+        <v>0.45895999999999998</v>
+      </c>
+      <c r="E12">
+        <v>0.76912999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>0.76644999999999996</v>
+      </c>
+      <c r="B13">
+        <v>0.72635000000000005</v>
+      </c>
+      <c r="C13">
+        <v>0.38603999999999999</v>
+      </c>
+      <c r="D13">
+        <v>0.64798999999999995</v>
+      </c>
+      <c r="E13">
+        <v>0.93440999999999996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>0.85592000000000001</v>
+      </c>
+      <c r="B14">
+        <v>0.28633999999999998</v>
+      </c>
+      <c r="C14">
+        <v>2.852E-2</v>
+      </c>
+      <c r="D14">
+        <v>0.75033000000000005</v>
+      </c>
+      <c r="E14">
+        <v>0.16582</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>0.83616999999999997</v>
+      </c>
+      <c r="B15">
+        <v>0.23338</v>
+      </c>
+      <c r="C15">
+        <v>0.31281999999999999</v>
+      </c>
+      <c r="D15">
+        <v>0.37685999999999997</v>
+      </c>
+      <c r="E15">
+        <v>0.24265</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>0.41126000000000001</v>
+      </c>
+      <c r="B16">
+        <v>0.12496</v>
+      </c>
+      <c r="C16">
+        <v>0.26255000000000001</v>
+      </c>
+      <c r="D16">
+        <v>0.14774999999999999</v>
+      </c>
+      <c r="E16">
+        <v>0.33838000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>0.29435</v>
+      </c>
+      <c r="B17">
+        <v>0.33107999999999999</v>
+      </c>
+      <c r="C17">
+        <v>0.63988</v>
+      </c>
+      <c r="D17">
+        <v>0.52309000000000005</v>
+      </c>
+      <c r="E17">
+        <v>0.79898000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>0.15973000000000001</v>
+      </c>
+      <c r="B18">
+        <v>0.25816</v>
+      </c>
+      <c r="C18">
+        <v>9.5649999999999999E-2</v>
+      </c>
+      <c r="D18">
+        <v>0.25264999999999999</v>
+      </c>
+      <c r="E18">
+        <v>0.69567999999999997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>0.96899999999999997</v>
+      </c>
+      <c r="B19">
+        <v>0.32417000000000001</v>
+      </c>
+      <c r="C19">
+        <v>0.33085999999999999</v>
+      </c>
+      <c r="D19">
+        <v>0.56032000000000004</v>
+      </c>
+      <c r="E19">
+        <v>0.18698999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>0.62411000000000005</v>
+      </c>
+      <c r="B20">
+        <v>0.82240000000000002</v>
+      </c>
+      <c r="C20">
+        <v>0.36007</v>
+      </c>
+      <c r="D20">
+        <v>0.89590000000000003</v>
+      </c>
+      <c r="E20">
+        <v>0.90139999999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>0.63048999999999999</v>
+      </c>
+      <c r="B21">
+        <v>0.25719999999999998</v>
+      </c>
+      <c r="C21">
+        <v>0.39816000000000001</v>
+      </c>
+      <c r="D21">
+        <v>0.95126999999999995</v>
+      </c>
+      <c r="E21">
+        <v>0.23269000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>0.29586000000000001</v>
+      </c>
+      <c r="B22">
+        <v>0.56733999999999996</v>
+      </c>
+      <c r="C22">
+        <v>0.10943</v>
+      </c>
+      <c r="D22">
+        <v>7.0029999999999995E-2</v>
+      </c>
+      <c r="E22">
+        <v>0.89188000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>0.10659</v>
+      </c>
+      <c r="B23">
+        <v>0.29458000000000001</v>
+      </c>
+      <c r="C23">
+        <v>0.22020000000000001</v>
+      </c>
+      <c r="D23">
+        <v>0.74611000000000005</v>
+      </c>
+      <c r="E23">
+        <v>0.49695</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>0.11703</v>
+      </c>
+      <c r="B24">
+        <v>0.29785</v>
+      </c>
+      <c r="C24">
+        <v>2.1010000000000001E-2</v>
+      </c>
+      <c r="D24">
+        <v>0.18756999999999999</v>
+      </c>
+      <c r="E24">
+        <v>0.38128000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>0.62348000000000003</v>
+      </c>
+      <c r="B25">
+        <v>0.63322000000000001</v>
+      </c>
+      <c r="C25">
+        <v>8.5419999999999996E-2</v>
+      </c>
+      <c r="D25">
+        <v>0.97141999999999995</v>
+      </c>
+      <c r="E25">
+        <v>0.29886000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>0.18276999999999999</v>
+      </c>
+      <c r="B26">
+        <v>0.37678</v>
+      </c>
+      <c r="C26">
+        <v>0.95482999999999996</v>
+      </c>
+      <c r="D26">
+        <v>0.55113000000000001</v>
+      </c>
+      <c r="E26">
+        <v>0.48133999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <f>AVERAGE(A1:A26)</f>
+        <v>0.54038923076923073</v>
+      </c>
+      <c r="B28">
+        <f t="shared" ref="B28:E28" si="0">AVERAGE(B1:B26)</f>
+        <v>0.3624373076923077</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>0.31629807692307704</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>0.4731653846153846</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>0.54797730769230768</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I218"/>
   <sheetViews>
-    <sheetView topLeftCell="A203" workbookViewId="0">
+    <sheetView topLeftCell="A201" workbookViewId="0">
       <selection activeCell="C236" sqref="C236"/>
     </sheetView>
   </sheetViews>
@@ -49503,8 +50035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L11" sqref="L11:T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -49538,7 +50070,7 @@
         <v>0.48398000000000002</v>
       </c>
       <c r="J1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
@@ -49570,7 +50102,7 @@
         <v>0.86477999999999999</v>
       </c>
       <c r="J2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
@@ -49605,7 +50137,7 @@
         <v>22</v>
       </c>
       <c r="K3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
@@ -49637,7 +50169,7 @@
         <v>0.13402</v>
       </c>
       <c r="J4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
@@ -49669,7 +50201,7 @@
         <v>0.28877999999999998</v>
       </c>
       <c r="J5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
@@ -49701,7 +50233,7 @@
         <v>0.58421999999999996</v>
       </c>
       <c r="J6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
@@ -49733,7 +50265,7 @@
         <v>0.78908999999999996</v>
       </c>
       <c r="J7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
@@ -49768,7 +50300,7 @@
         <v>22</v>
       </c>
       <c r="K8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L8">
         <v>0.61297999999999997</v>
@@ -49827,10 +50359,10 @@
         <v>0.7611</v>
       </c>
       <c r="J9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L9">
         <v>0.61245000000000005</v>
@@ -49889,7 +50421,7 @@
         <v>0.67276000000000002</v>
       </c>
       <c r="J10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="L10">
         <v>0.85077000000000003</v>
@@ -49948,7 +50480,7 @@
         <v>0.56696999999999997</v>
       </c>
       <c r="J11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L11">
         <v>0.37486000000000003</v>
@@ -50007,7 +50539,7 @@
         <v>4.3909999999999998E-2</v>
       </c>
       <c r="J12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="L12">
         <v>0.40176000000000001</v>
@@ -50069,7 +50601,7 @@
         <v>22</v>
       </c>
       <c r="K13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L13">
         <v>0.1081</v>
@@ -50128,7 +50660,7 @@
         <v>0.77242999999999995</v>
       </c>
       <c r="J14" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
@@ -50163,7 +50695,7 @@
         <v>22</v>
       </c>
       <c r="K15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L15">
         <f>AVERAGE(L8:L13)</f>
@@ -50198,7 +50730,7 @@
         <v>0.35705333333333339</v>
       </c>
       <c r="T15">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(T8:T13)</f>
         <v>0.69429833333333324</v>
       </c>
     </row>
@@ -50234,7 +50766,7 @@
         <v>22</v>
       </c>
       <c r="K16" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
@@ -50266,7 +50798,7 @@
         <v>0.82791000000000003</v>
       </c>
       <c r="J17" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
@@ -50298,7 +50830,7 @@
         <v>0.48319000000000001</v>
       </c>
       <c r="J18" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
@@ -50330,13 +50862,3221 @@
         <v>0.57240999999999997</v>
       </c>
       <c r="J19" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K19" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H74"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M35" sqref="M35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="5" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>0.59172000000000002</v>
+      </c>
+      <c r="B1">
+        <v>0.95459000000000005</v>
+      </c>
+      <c r="C1">
+        <v>0.78922000000000003</v>
+      </c>
+      <c r="D1">
+        <v>0.59816000000000003</v>
+      </c>
+      <c r="E1">
+        <v>0.10668999999999999</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>3.4700000000000002E-2</v>
+      </c>
+      <c r="B2">
+        <v>0.77490000000000003</v>
+      </c>
+      <c r="C2">
+        <v>0.22144</v>
+      </c>
+      <c r="D2">
+        <v>0.93357000000000001</v>
+      </c>
+      <c r="E2">
+        <v>0.21929999999999999</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>0.46506999999999998</v>
+      </c>
+      <c r="B3">
+        <v>0.46631</v>
+      </c>
+      <c r="C3">
+        <v>0.99619000000000002</v>
+      </c>
+      <c r="D3">
+        <v>0.84853999999999996</v>
+      </c>
+      <c r="E3">
+        <v>0.19222</v>
+      </c>
+      <c r="F3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>0.60641</v>
+      </c>
+      <c r="B4">
+        <v>0.56093999999999999</v>
+      </c>
+      <c r="C4">
+        <v>0.81496999999999997</v>
+      </c>
+      <c r="D4">
+        <v>0.81389</v>
+      </c>
+      <c r="E4">
+        <v>0.20175999999999999</v>
+      </c>
+      <c r="F4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>0.18315000000000001</v>
+      </c>
+      <c r="B5">
+        <v>0.43090000000000001</v>
+      </c>
+      <c r="C5">
+        <v>0.16844000000000001</v>
+      </c>
+      <c r="D5">
+        <v>0.44259999999999999</v>
+      </c>
+      <c r="E5">
+        <v>0.26811000000000001</v>
+      </c>
+      <c r="F5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>0.41105000000000003</v>
+      </c>
+      <c r="B6">
+        <v>0.75553000000000003</v>
+      </c>
+      <c r="C6">
+        <v>0.74789000000000005</v>
+      </c>
+      <c r="D6">
+        <v>0.16002</v>
+      </c>
+      <c r="E6">
+        <v>0.18848000000000001</v>
+      </c>
+      <c r="F6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>0.29805999999999999</v>
+      </c>
+      <c r="B7">
+        <v>0.54944999999999999</v>
+      </c>
+      <c r="C7">
+        <v>0.74207000000000001</v>
+      </c>
+      <c r="D7">
+        <v>0.71531999999999996</v>
+      </c>
+      <c r="E7">
+        <v>0.38669999999999999</v>
+      </c>
+      <c r="F7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>0.40611000000000003</v>
+      </c>
+      <c r="B8">
+        <v>0.71838999999999997</v>
+      </c>
+      <c r="C8">
+        <v>0.87339999999999995</v>
+      </c>
+      <c r="D8">
+        <v>0.55533999999999994</v>
+      </c>
+      <c r="E8">
+        <v>0.41875000000000001</v>
+      </c>
+      <c r="F8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>0.75077000000000005</v>
+      </c>
+      <c r="B9">
+        <v>0.97882999999999998</v>
+      </c>
+      <c r="C9">
+        <v>0.43187999999999999</v>
+      </c>
+      <c r="D9">
+        <v>0.31391999999999998</v>
+      </c>
+      <c r="E9">
+        <v>0.63036000000000003</v>
+      </c>
+      <c r="F9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>0.11117</v>
+      </c>
+      <c r="B10">
+        <v>0.72433000000000003</v>
+      </c>
+      <c r="C10">
+        <v>0.67215999999999998</v>
+      </c>
+      <c r="D10">
+        <v>0.64409000000000005</v>
+      </c>
+      <c r="E10">
+        <v>0.19605</v>
+      </c>
+      <c r="F10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>0.56923000000000001</v>
+      </c>
+      <c r="B11">
+        <v>0.73446</v>
+      </c>
+      <c r="C11">
+        <v>0.35820000000000002</v>
+      </c>
+      <c r="D11">
+        <v>0.88456999999999997</v>
+      </c>
+      <c r="E11">
+        <v>0.18923000000000001</v>
+      </c>
+      <c r="F11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>0.16022</v>
+      </c>
+      <c r="B12">
+        <v>0.95938000000000001</v>
+      </c>
+      <c r="C12">
+        <v>0.56166000000000005</v>
+      </c>
+      <c r="D12">
+        <v>0.96994000000000002</v>
+      </c>
+      <c r="E12">
+        <v>6.0940000000000001E-2</v>
+      </c>
+      <c r="F12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>0.95806000000000002</v>
+      </c>
+      <c r="B13">
+        <v>0.89353000000000005</v>
+      </c>
+      <c r="C13">
+        <v>3.499E-2</v>
+      </c>
+      <c r="D13">
+        <v>0.97674000000000005</v>
+      </c>
+      <c r="E13">
+        <v>4.9300000000000004E-3</v>
+      </c>
+      <c r="F13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>0.48182999999999998</v>
+      </c>
+      <c r="B14">
+        <v>0.73953000000000002</v>
+      </c>
+      <c r="C14">
+        <v>0.34666000000000002</v>
+      </c>
+      <c r="D14">
+        <v>0.62787000000000004</v>
+      </c>
+      <c r="E14">
+        <v>0.24013000000000001</v>
+      </c>
+      <c r="F14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>0.41491</v>
+      </c>
+      <c r="B15">
+        <v>0.99336999999999998</v>
+      </c>
+      <c r="C15">
+        <v>0.76380999999999999</v>
+      </c>
+      <c r="D15">
+        <v>0.59904999999999997</v>
+      </c>
+      <c r="E15">
+        <v>0.60606000000000004</v>
+      </c>
+      <c r="F15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>0.15467</v>
+      </c>
+      <c r="B16">
+        <v>7.9369999999999996E-2</v>
+      </c>
+      <c r="C16">
+        <v>0.89478999999999997</v>
+      </c>
+      <c r="D16">
+        <v>0.34</v>
+      </c>
+      <c r="E16">
+        <v>0.10739</v>
+      </c>
+      <c r="F16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>0.67027999999999999</v>
+      </c>
+      <c r="B17">
+        <v>0.60572999999999999</v>
+      </c>
+      <c r="C17">
+        <v>0.36503999999999998</v>
+      </c>
+      <c r="D17">
+        <v>7.5039999999999996E-2</v>
+      </c>
+      <c r="E17">
+        <v>0.20527999999999999</v>
+      </c>
+      <c r="F17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>0.85843000000000003</v>
+      </c>
+      <c r="B18">
+        <v>0.34379999999999999</v>
+      </c>
+      <c r="C18">
+        <v>0.92222000000000004</v>
+      </c>
+      <c r="D18">
+        <v>0.36463000000000001</v>
+      </c>
+      <c r="E18">
+        <v>0.27017999999999998</v>
+      </c>
+      <c r="F18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>0.89126000000000005</v>
+      </c>
+      <c r="B19">
+        <v>0.11559</v>
+      </c>
+      <c r="C19">
+        <v>0.87597999999999998</v>
+      </c>
+      <c r="D19">
+        <v>0.39267999999999997</v>
+      </c>
+      <c r="E19">
+        <v>0.42520999999999998</v>
+      </c>
+      <c r="F19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>0.87280000000000002</v>
+      </c>
+      <c r="B20">
+        <v>0.76995999999999998</v>
+      </c>
+      <c r="C20">
+        <v>0.13012000000000001</v>
+      </c>
+      <c r="D20">
+        <v>0.15334999999999999</v>
+      </c>
+      <c r="E20">
+        <v>0.22538</v>
+      </c>
+      <c r="F20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>0.96892</v>
+      </c>
+      <c r="B21">
+        <v>0.19183</v>
+      </c>
+      <c r="C21">
+        <v>2.6249999999999999E-2</v>
+      </c>
+      <c r="D21">
+        <v>0.71174999999999999</v>
+      </c>
+      <c r="E21">
+        <v>0.52393999999999996</v>
+      </c>
+      <c r="F21" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>0.24013000000000001</v>
+      </c>
+      <c r="B22">
+        <v>0.97635000000000005</v>
+      </c>
+      <c r="C22">
+        <v>0.61939</v>
+      </c>
+      <c r="D22">
+        <v>0.79698999999999998</v>
+      </c>
+      <c r="E22">
+        <v>0.57330999999999999</v>
+      </c>
+      <c r="F22" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>0.31058999999999998</v>
+      </c>
+      <c r="B23">
+        <v>0.95982999999999996</v>
+      </c>
+      <c r="C23">
+        <v>0.89981999999999995</v>
+      </c>
+      <c r="D23">
+        <v>0.27911000000000002</v>
+      </c>
+      <c r="E23">
+        <v>1.193E-2</v>
+      </c>
+      <c r="F23" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>0.79951000000000005</v>
+      </c>
+      <c r="B24">
+        <v>0.88141000000000003</v>
+      </c>
+      <c r="C24">
+        <v>0.48016999999999999</v>
+      </c>
+      <c r="D24">
+        <v>0.86141000000000001</v>
+      </c>
+      <c r="E24">
+        <v>0.99355000000000004</v>
+      </c>
+      <c r="F24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>6.5360000000000001E-2</v>
+      </c>
+      <c r="B25">
+        <v>3.9030000000000002E-2</v>
+      </c>
+      <c r="C25">
+        <v>0.29492000000000002</v>
+      </c>
+      <c r="D25">
+        <v>0.32332</v>
+      </c>
+      <c r="E25">
+        <v>0.46206000000000003</v>
+      </c>
+      <c r="F25" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>0.10655000000000001</v>
+      </c>
+      <c r="B26">
+        <v>0.50180000000000002</v>
+      </c>
+      <c r="C26">
+        <v>0.66105000000000003</v>
+      </c>
+      <c r="D26">
+        <v>0.44894000000000001</v>
+      </c>
+      <c r="E26">
+        <v>0.49656</v>
+      </c>
+      <c r="F26" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>7.1040000000000006E-2</v>
+      </c>
+      <c r="B27">
+        <v>0.80349000000000004</v>
+      </c>
+      <c r="C27">
+        <v>0.49880999999999998</v>
+      </c>
+      <c r="D27">
+        <v>0.48087999999999997</v>
+      </c>
+      <c r="E27">
+        <v>0.51351999999999998</v>
+      </c>
+      <c r="F27" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>0.38096000000000002</v>
+      </c>
+      <c r="B28">
+        <v>1.422E-2</v>
+      </c>
+      <c r="C28">
+        <v>0.58013999999999999</v>
+      </c>
+      <c r="D28">
+        <v>0.34025</v>
+      </c>
+      <c r="E28">
+        <v>0.13499</v>
+      </c>
+      <c r="F28" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>0.72767999999999999</v>
+      </c>
+      <c r="B29">
+        <v>0.46422000000000002</v>
+      </c>
+      <c r="C29">
+        <v>0.66788999999999998</v>
+      </c>
+      <c r="D29">
+        <v>0.5071</v>
+      </c>
+      <c r="E29">
+        <v>0.73851999999999995</v>
+      </c>
+      <c r="F29" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>0.59823999999999999</v>
+      </c>
+      <c r="B30">
+        <v>0.21368000000000001</v>
+      </c>
+      <c r="C30">
+        <v>0.30726999999999999</v>
+      </c>
+      <c r="D30">
+        <v>0.83357999999999999</v>
+      </c>
+      <c r="E30">
+        <v>0.51790999999999998</v>
+      </c>
+      <c r="F30" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>1.115E-2</v>
+      </c>
+      <c r="B31">
+        <v>0.15262999999999999</v>
+      </c>
+      <c r="C31">
+        <v>7.4139999999999998E-2</v>
+      </c>
+      <c r="D31">
+        <v>0.61426000000000003</v>
+      </c>
+      <c r="E31">
+        <v>0.20852999999999999</v>
+      </c>
+      <c r="F31" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>0.21228</v>
+      </c>
+      <c r="B32">
+        <v>0.11672</v>
+      </c>
+      <c r="C32">
+        <v>0.64603999999999995</v>
+      </c>
+      <c r="D32">
+        <v>0.34079999999999999</v>
+      </c>
+      <c r="E32">
+        <v>0.61102000000000001</v>
+      </c>
+      <c r="F32" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>0.57806000000000002</v>
+      </c>
+      <c r="B33">
+        <v>0.31341000000000002</v>
+      </c>
+      <c r="C33">
+        <v>0.25163000000000002</v>
+      </c>
+      <c r="D33">
+        <v>0.87226999999999999</v>
+      </c>
+      <c r="E33">
+        <v>0.51931000000000005</v>
+      </c>
+      <c r="F33" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>0.65376999999999996</v>
+      </c>
+      <c r="B34">
+        <v>0.30512</v>
+      </c>
+      <c r="C34">
+        <v>0.17293</v>
+      </c>
+      <c r="D34">
+        <v>0.87143000000000004</v>
+      </c>
+      <c r="E34">
+        <v>0.64885999999999999</v>
+      </c>
+      <c r="F34" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>0.20752000000000001</v>
+      </c>
+      <c r="B35">
+        <v>0.84245000000000003</v>
+      </c>
+      <c r="C35">
+        <v>0.51295999999999997</v>
+      </c>
+      <c r="D35">
+        <v>0.73046999999999995</v>
+      </c>
+      <c r="E35">
+        <v>0.58694999999999997</v>
+      </c>
+      <c r="F35" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>0.22861999999999999</v>
+      </c>
+      <c r="B36">
+        <v>0.49275999999999998</v>
+      </c>
+      <c r="C36">
+        <v>0.57730999999999999</v>
+      </c>
+      <c r="D36">
+        <v>0.27615000000000001</v>
+      </c>
+      <c r="E36">
+        <v>0.87483</v>
+      </c>
+      <c r="F36" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>0.77668000000000004</v>
+      </c>
+      <c r="B37">
+        <v>0.25847999999999999</v>
+      </c>
+      <c r="C37">
+        <v>2.903E-2</v>
+      </c>
+      <c r="D37">
+        <v>0.67742000000000002</v>
+      </c>
+      <c r="E37">
+        <v>0.52483000000000002</v>
+      </c>
+      <c r="F37" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>0.9556</v>
+      </c>
+      <c r="B38">
+        <v>0.70899000000000001</v>
+      </c>
+      <c r="C38">
+        <v>0.61163999999999996</v>
+      </c>
+      <c r="D38">
+        <v>0.58655000000000002</v>
+      </c>
+      <c r="E38">
+        <v>0.91615000000000002</v>
+      </c>
+      <c r="F38" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>0.94520000000000004</v>
+      </c>
+      <c r="B39">
+        <v>0.77297000000000005</v>
+      </c>
+      <c r="C39">
+        <v>6.2820000000000001E-2</v>
+      </c>
+      <c r="D39">
+        <v>0.96084999999999998</v>
+      </c>
+      <c r="E39">
+        <v>0.91835999999999995</v>
+      </c>
+      <c r="F39" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>0.27816999999999997</v>
+      </c>
+      <c r="B40">
+        <v>0.18831999999999999</v>
+      </c>
+      <c r="C40">
+        <v>0.39479999999999998</v>
+      </c>
+      <c r="D40">
+        <v>0.74883</v>
+      </c>
+      <c r="E40">
+        <v>0.79166999999999998</v>
+      </c>
+      <c r="F40" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>0.77554999999999996</v>
+      </c>
+      <c r="B41">
+        <v>0.63358999999999999</v>
+      </c>
+      <c r="C41">
+        <v>9.9879999999999997E-2</v>
+      </c>
+      <c r="D41">
+        <v>0.68171000000000004</v>
+      </c>
+      <c r="E41">
+        <v>0.46353</v>
+      </c>
+      <c r="F41" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>0.70262000000000002</v>
+      </c>
+      <c r="B42">
+        <v>0.80271000000000003</v>
+      </c>
+      <c r="C42">
+        <v>0.34405000000000002</v>
+      </c>
+      <c r="D42">
+        <v>0.93859999999999999</v>
+      </c>
+      <c r="E42">
+        <v>4.3400000000000001E-3</v>
+      </c>
+      <c r="F42" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>0.90790999999999999</v>
+      </c>
+      <c r="B43">
+        <v>0.67545999999999995</v>
+      </c>
+      <c r="C43">
+        <v>0.85655000000000003</v>
+      </c>
+      <c r="D43">
+        <v>0.15661</v>
+      </c>
+      <c r="E43">
+        <v>0.73990999999999996</v>
+      </c>
+      <c r="F43" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>0.45655000000000001</v>
+      </c>
+      <c r="B44">
+        <v>0.4294</v>
+      </c>
+      <c r="C44">
+        <v>0.59740000000000004</v>
+      </c>
+      <c r="D44">
+        <v>0.29677999999999999</v>
+      </c>
+      <c r="E44">
+        <v>0.32164999999999999</v>
+      </c>
+      <c r="F44" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>0.74339999999999995</v>
+      </c>
+      <c r="B45">
+        <v>0.18573000000000001</v>
+      </c>
+      <c r="C45">
+        <v>0.75485000000000002</v>
+      </c>
+      <c r="D45">
+        <v>0.85682000000000003</v>
+      </c>
+      <c r="E45">
+        <v>0.68291000000000002</v>
+      </c>
+      <c r="F45" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>0.83140000000000003</v>
+      </c>
+      <c r="B46">
+        <v>0.25725999999999999</v>
+      </c>
+      <c r="C46">
+        <v>9.2469999999999997E-2</v>
+      </c>
+      <c r="D46">
+        <v>0.41744999999999999</v>
+      </c>
+      <c r="E46">
+        <v>0.9052</v>
+      </c>
+      <c r="F46" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>0.35319</v>
+      </c>
+      <c r="B47">
+        <v>7.1209999999999996E-2</v>
+      </c>
+      <c r="C47">
+        <v>0.87307000000000001</v>
+      </c>
+      <c r="D47">
+        <v>0.84275999999999995</v>
+      </c>
+      <c r="E47">
+        <v>0.35616999999999999</v>
+      </c>
+      <c r="F47" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>0.36697999999999997</v>
+      </c>
+      <c r="B48">
+        <v>9.672E-2</v>
+      </c>
+      <c r="C48">
+        <v>0.14985000000000001</v>
+      </c>
+      <c r="D48">
+        <v>3.6769999999999997E-2</v>
+      </c>
+      <c r="E48">
+        <v>0.44023000000000001</v>
+      </c>
+      <c r="F48" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>0.89932000000000001</v>
+      </c>
+      <c r="B49">
+        <v>0.83962999999999999</v>
+      </c>
+      <c r="C49">
+        <v>0.55303000000000002</v>
+      </c>
+      <c r="D49">
+        <v>0.98553000000000002</v>
+      </c>
+      <c r="E49">
+        <v>0.68740000000000001</v>
+      </c>
+      <c r="F49" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>0.89636000000000005</v>
+      </c>
+      <c r="B50">
+        <v>0.91237000000000001</v>
+      </c>
+      <c r="C50">
+        <v>0.76337999999999995</v>
+      </c>
+      <c r="D50">
+        <v>0.48982999999999999</v>
+      </c>
+      <c r="E50">
+        <v>0.34299000000000002</v>
+      </c>
+      <c r="F50" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>0.61858999999999997</v>
+      </c>
+      <c r="B51">
+        <v>0.40687000000000001</v>
+      </c>
+      <c r="C51">
+        <v>0.19209999999999999</v>
+      </c>
+      <c r="D51">
+        <v>0.26928999999999997</v>
+      </c>
+      <c r="E51">
+        <v>0.25105</v>
+      </c>
+      <c r="F51" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>0.31746000000000002</v>
+      </c>
+      <c r="B52">
+        <v>0.69825999999999999</v>
+      </c>
+      <c r="C52">
+        <v>0.30782999999999999</v>
+      </c>
+      <c r="D52">
+        <v>0.79906999999999995</v>
+      </c>
+      <c r="E52">
+        <v>0.93088000000000004</v>
+      </c>
+      <c r="F52" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>0.56659999999999999</v>
+      </c>
+      <c r="B53">
+        <v>0.44969999999999999</v>
+      </c>
+      <c r="C53">
+        <v>0.55089999999999995</v>
+      </c>
+      <c r="D53">
+        <v>0.22741</v>
+      </c>
+      <c r="E53">
+        <v>8.7980000000000003E-2</v>
+      </c>
+      <c r="F53" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>0.97372999999999998</v>
+      </c>
+      <c r="B54">
+        <v>0.67206999999999995</v>
+      </c>
+      <c r="C54">
+        <v>0.72702999999999995</v>
+      </c>
+      <c r="D54">
+        <v>0.43581999999999999</v>
+      </c>
+      <c r="E54">
+        <v>0.17516000000000001</v>
+      </c>
+      <c r="F54" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>0.14526</v>
+      </c>
+      <c r="B55">
+        <v>0.81459000000000004</v>
+      </c>
+      <c r="C55">
+        <v>0.73490999999999995</v>
+      </c>
+      <c r="D55">
+        <v>0.36485000000000001</v>
+      </c>
+      <c r="E55">
+        <v>0.59206999999999999</v>
+      </c>
+      <c r="F55" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>0.96957000000000004</v>
+      </c>
+      <c r="B56">
+        <v>0.51114000000000004</v>
+      </c>
+      <c r="C56">
+        <v>0.95389999999999997</v>
+      </c>
+      <c r="D56">
+        <v>0.61099999999999999</v>
+      </c>
+      <c r="E56">
+        <v>0.57599999999999996</v>
+      </c>
+      <c r="F56" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>0.41972999999999999</v>
+      </c>
+      <c r="B57">
+        <v>0.49867</v>
+      </c>
+      <c r="C57">
+        <v>0.25481999999999999</v>
+      </c>
+      <c r="D57">
+        <v>0.89549000000000001</v>
+      </c>
+      <c r="E57">
+        <v>0.99536999999999998</v>
+      </c>
+      <c r="F57" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>0.9869</v>
+      </c>
+      <c r="B58">
+        <v>0.11359</v>
+      </c>
+      <c r="C58">
+        <v>6.8599999999999994E-2</v>
+      </c>
+      <c r="D58">
+        <v>0.35615999999999998</v>
+      </c>
+      <c r="E58">
+        <v>0.10253</v>
+      </c>
+      <c r="F58" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>0.29150999999999999</v>
+      </c>
+      <c r="B59">
+        <v>0.48348000000000002</v>
+      </c>
+      <c r="C59">
+        <v>0.23402000000000001</v>
+      </c>
+      <c r="D59">
+        <v>1.404E-2</v>
+      </c>
+      <c r="E59">
+        <v>0.81486000000000003</v>
+      </c>
+      <c r="F59" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>0.77346999999999999</v>
+      </c>
+      <c r="B60">
+        <v>0.76761000000000001</v>
+      </c>
+      <c r="C60">
+        <v>0.23537</v>
+      </c>
+      <c r="D60">
+        <v>0.72043999999999997</v>
+      </c>
+      <c r="E60">
+        <v>0.94328000000000001</v>
+      </c>
+      <c r="F60" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>0.78979999999999995</v>
+      </c>
+      <c r="B61">
+        <v>0.65200000000000002</v>
+      </c>
+      <c r="C61">
+        <v>0.85675999999999997</v>
+      </c>
+      <c r="D61">
+        <v>0.33894999999999997</v>
+      </c>
+      <c r="E61">
+        <v>0.45779999999999998</v>
+      </c>
+      <c r="F61" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>0.29203000000000001</v>
+      </c>
+      <c r="B62">
+        <v>0.13503000000000001</v>
+      </c>
+      <c r="C62">
+        <v>0.1804</v>
+      </c>
+      <c r="D62">
+        <v>0.41471999999999998</v>
+      </c>
+      <c r="E62">
+        <v>0.86631999999999998</v>
+      </c>
+      <c r="F62" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>0.90817999999999999</v>
+      </c>
+      <c r="B63">
+        <v>0.82757000000000003</v>
+      </c>
+      <c r="C63">
+        <v>0.33929999999999999</v>
+      </c>
+      <c r="D63">
+        <v>0.71919</v>
+      </c>
+      <c r="E63">
+        <v>0.62597000000000003</v>
+      </c>
+      <c r="F63" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>0.51775000000000004</v>
+      </c>
+      <c r="B64">
+        <v>0.80991999999999997</v>
+      </c>
+      <c r="C64">
+        <v>0.59960000000000002</v>
+      </c>
+      <c r="D64">
+        <v>0.52661000000000002</v>
+      </c>
+      <c r="E64">
+        <v>0.96145999999999998</v>
+      </c>
+      <c r="F64" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>0.98063</v>
+      </c>
+      <c r="B65">
+        <v>0.24773999999999999</v>
+      </c>
+      <c r="C65">
+        <v>0.33845999999999998</v>
+      </c>
+      <c r="D65">
+        <v>0.85004999999999997</v>
+      </c>
+      <c r="E65">
+        <v>0.43424000000000001</v>
+      </c>
+      <c r="F65" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>0.43547999999999998</v>
+      </c>
+      <c r="B66">
+        <v>0.93337000000000003</v>
+      </c>
+      <c r="C66">
+        <v>0.47326000000000001</v>
+      </c>
+      <c r="D66">
+        <v>0.15029000000000001</v>
+      </c>
+      <c r="E66">
+        <v>0.26801000000000003</v>
+      </c>
+      <c r="F66" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>0.17488000000000001</v>
+      </c>
+      <c r="B67">
+        <v>0.84584000000000004</v>
+      </c>
+      <c r="C67">
+        <v>0.76898</v>
+      </c>
+      <c r="D67">
+        <v>0.92691000000000001</v>
+      </c>
+      <c r="E67">
+        <v>0.78691999999999995</v>
+      </c>
+      <c r="F67" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>0.93457000000000001</v>
+      </c>
+      <c r="B68">
+        <v>0.13211000000000001</v>
+      </c>
+      <c r="C68">
+        <v>0.18089</v>
+      </c>
+      <c r="D68">
+        <v>0.93918999999999997</v>
+      </c>
+      <c r="E68">
+        <v>0.49642999999999998</v>
+      </c>
+      <c r="F68" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>0.25369999999999998</v>
+      </c>
+      <c r="B69">
+        <v>0.94081000000000004</v>
+      </c>
+      <c r="C69">
+        <v>0.24088999999999999</v>
+      </c>
+      <c r="D69">
+        <v>0.97748000000000002</v>
+      </c>
+      <c r="E69">
+        <v>0.82676000000000005</v>
+      </c>
+      <c r="F69" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>0.94616999999999996</v>
+      </c>
+      <c r="B70">
+        <v>0.30957000000000001</v>
+      </c>
+      <c r="C70">
+        <v>0.12232</v>
+      </c>
+      <c r="D70">
+        <v>0.37586999999999998</v>
+      </c>
+      <c r="E70">
+        <v>0.19359999999999999</v>
+      </c>
+      <c r="F70" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>0.12756000000000001</v>
+      </c>
+      <c r="B71">
+        <v>3.2439999999999997E-2</v>
+      </c>
+      <c r="C71">
+        <v>0.83579000000000003</v>
+      </c>
+      <c r="D71">
+        <v>0.89763999999999999</v>
+      </c>
+      <c r="E71">
+        <v>0.52351000000000003</v>
+      </c>
+      <c r="F71" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>5.1270000000000003E-2</v>
+      </c>
+      <c r="B72">
+        <v>0.34476000000000001</v>
+      </c>
+      <c r="C72">
+        <v>0.62836999999999998</v>
+      </c>
+      <c r="D72">
+        <v>4.8239999999999998E-2</v>
+      </c>
+      <c r="E72">
+        <v>0.72062000000000004</v>
+      </c>
+      <c r="F72" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>0.50555000000000005</v>
+      </c>
+      <c r="B73">
+        <v>6.6830000000000001E-2</v>
+      </c>
+      <c r="C73">
+        <v>0.22988</v>
+      </c>
+      <c r="D73">
+        <v>0.85033000000000003</v>
+      </c>
+      <c r="E73">
+        <v>0.23365</v>
+      </c>
+      <c r="F73" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>0.86767000000000005</v>
+      </c>
+      <c r="B74">
+        <v>0.89183000000000001</v>
+      </c>
+      <c r="C74">
+        <v>0.48623</v>
+      </c>
+      <c r="D74">
+        <v>0.47602</v>
+      </c>
+      <c r="E74">
+        <v>0.80056000000000005</v>
+      </c>
+      <c r="F74" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A1:F74">
+    <sortCondition ref="F1:F74"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:E23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>3.4700000000000002E-2</v>
+      </c>
+      <c r="B1">
+        <v>0.77490000000000003</v>
+      </c>
+      <c r="C1">
+        <v>0.22144</v>
+      </c>
+      <c r="D1">
+        <v>0.93357000000000001</v>
+      </c>
+      <c r="E1">
+        <v>0.21929999999999999</v>
+      </c>
+      <c r="F1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0.46506999999999998</v>
+      </c>
+      <c r="B2">
+        <v>0.46631</v>
+      </c>
+      <c r="C2">
+        <v>0.99619000000000002</v>
+      </c>
+      <c r="D2">
+        <v>0.84853999999999996</v>
+      </c>
+      <c r="E2">
+        <v>0.19222</v>
+      </c>
+      <c r="F2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>0.60641</v>
+      </c>
+      <c r="B3">
+        <v>0.56093999999999999</v>
+      </c>
+      <c r="C3">
+        <v>0.81496999999999997</v>
+      </c>
+      <c r="D3">
+        <v>0.81389</v>
+      </c>
+      <c r="E3">
+        <v>0.20175999999999999</v>
+      </c>
+      <c r="F3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>0.18315000000000001</v>
+      </c>
+      <c r="B4">
+        <v>0.43090000000000001</v>
+      </c>
+      <c r="C4">
+        <v>0.16844000000000001</v>
+      </c>
+      <c r="D4">
+        <v>0.44259999999999999</v>
+      </c>
+      <c r="E4">
+        <v>0.26811000000000001</v>
+      </c>
+      <c r="F4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>0.29805999999999999</v>
+      </c>
+      <c r="B5">
+        <v>0.54944999999999999</v>
+      </c>
+      <c r="C5">
+        <v>0.74207000000000001</v>
+      </c>
+      <c r="D5">
+        <v>0.71531999999999996</v>
+      </c>
+      <c r="E5">
+        <v>0.38669999999999999</v>
+      </c>
+      <c r="F5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>0.40611000000000003</v>
+      </c>
+      <c r="B6">
+        <v>0.71838999999999997</v>
+      </c>
+      <c r="C6">
+        <v>0.87339999999999995</v>
+      </c>
+      <c r="D6">
+        <v>0.55533999999999994</v>
+      </c>
+      <c r="E6">
+        <v>0.41875000000000001</v>
+      </c>
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>3.4700000000000002E-2</v>
+      </c>
+      <c r="B9">
+        <v>0.77490000000000003</v>
+      </c>
+      <c r="C9">
+        <v>0.22144</v>
+      </c>
+      <c r="D9">
+        <v>0.93357000000000001</v>
+      </c>
+      <c r="E9">
+        <v>0.21929999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>0.60641</v>
+      </c>
+      <c r="B10">
+        <v>0.56093999999999999</v>
+      </c>
+      <c r="C10">
+        <v>0.81496999999999997</v>
+      </c>
+      <c r="D10">
+        <v>0.81389</v>
+      </c>
+      <c r="E10">
+        <v>0.20175999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>0.18315000000000001</v>
+      </c>
+      <c r="B11">
+        <v>0.43090000000000001</v>
+      </c>
+      <c r="C11">
+        <v>0.16844000000000001</v>
+      </c>
+      <c r="D11">
+        <v>0.44259999999999999</v>
+      </c>
+      <c r="E11">
+        <v>0.26811000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>0.29805999999999999</v>
+      </c>
+      <c r="B12">
+        <v>0.54944999999999999</v>
+      </c>
+      <c r="C12">
+        <v>0.74207000000000001</v>
+      </c>
+      <c r="D12">
+        <v>0.71531999999999996</v>
+      </c>
+      <c r="E12">
+        <v>0.38669999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>0.40611000000000003</v>
+      </c>
+      <c r="B13">
+        <v>0.71838999999999997</v>
+      </c>
+      <c r="C13">
+        <v>0.87339999999999995</v>
+      </c>
+      <c r="D13">
+        <v>0.55533999999999994</v>
+      </c>
+      <c r="E13">
+        <v>0.41875000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <f>AVERAGE(A9:A13)</f>
+        <v>0.30568600000000001</v>
+      </c>
+      <c r="B15">
+        <f>AVERAGE(B9:B13)</f>
+        <v>0.60691600000000001</v>
+      </c>
+      <c r="C15">
+        <f>AVERAGE(C9:C13)</f>
+        <v>0.5640639999999999</v>
+      </c>
+      <c r="D15">
+        <f>AVERAGE(D9:D13)</f>
+        <v>0.69214400000000009</v>
+      </c>
+      <c r="E15">
+        <f>AVERAGE(E9:E13)</f>
+        <v>0.29892400000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>0.29805999999999999</v>
+      </c>
+      <c r="B23">
+        <v>0.54944999999999999</v>
+      </c>
+      <c r="C23">
+        <v>0.74207000000000001</v>
+      </c>
+      <c r="D23">
+        <v>0.71531999999999996</v>
+      </c>
+      <c r="E23">
+        <v>0.38669999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F69"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q29" sqref="K1:Q29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="5" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>0.99041999999999997</v>
+      </c>
+      <c r="B1">
+        <v>0.34425</v>
+      </c>
+      <c r="C1">
+        <v>0.74646999999999997</v>
+      </c>
+      <c r="D1">
+        <v>4.6640000000000001E-2</v>
+      </c>
+      <c r="E1">
+        <v>0.71260000000000001</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0.61282000000000003</v>
+      </c>
+      <c r="B2">
+        <v>0.32585999999999998</v>
+      </c>
+      <c r="C2">
+        <v>5.1189999999999999E-2</v>
+      </c>
+      <c r="D2">
+        <v>0.70777000000000001</v>
+      </c>
+      <c r="E2">
+        <v>0.74356999999999995</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>0.35022999999999999</v>
+      </c>
+      <c r="B3">
+        <v>0.15390000000000001</v>
+      </c>
+      <c r="C3">
+        <v>0.18507999999999999</v>
+      </c>
+      <c r="D3">
+        <v>0.43325999999999998</v>
+      </c>
+      <c r="E3">
+        <v>0.93557000000000001</v>
+      </c>
+      <c r="F3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>0.53010999999999997</v>
+      </c>
+      <c r="B4">
+        <v>0.23518</v>
+      </c>
+      <c r="C4">
+        <v>0.45567000000000002</v>
+      </c>
+      <c r="D4">
+        <v>0.36456</v>
+      </c>
+      <c r="E4">
+        <v>0.25274999999999997</v>
+      </c>
+      <c r="F4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>0.90078999999999998</v>
+      </c>
+      <c r="B5">
+        <v>6.1690000000000002E-2</v>
+      </c>
+      <c r="C5">
+        <v>0.16364999999999999</v>
+      </c>
+      <c r="D5">
+        <v>0.14494000000000001</v>
+      </c>
+      <c r="E5">
+        <v>0.70272999999999997</v>
+      </c>
+      <c r="F5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>6.9940000000000002E-2</v>
+      </c>
+      <c r="B6">
+        <v>3.0290000000000001E-2</v>
+      </c>
+      <c r="C6">
+        <v>0.10782</v>
+      </c>
+      <c r="D6">
+        <v>0.14846000000000001</v>
+      </c>
+      <c r="E6">
+        <v>2.7060000000000001E-2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>0.79744000000000004</v>
+      </c>
+      <c r="B7">
+        <v>0.93918999999999997</v>
+      </c>
+      <c r="C7">
+        <v>0.24818000000000001</v>
+      </c>
+      <c r="D7">
+        <v>0.20507</v>
+      </c>
+      <c r="E7">
+        <v>0.83004</v>
+      </c>
+      <c r="F7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>0.71872000000000003</v>
+      </c>
+      <c r="B8">
+        <v>1.9279999999999999E-2</v>
+      </c>
+      <c r="C8">
+        <v>0.30670999999999998</v>
+      </c>
+      <c r="D8">
+        <v>8.5629999999999998E-2</v>
+      </c>
+      <c r="E8">
+        <v>0.15526999999999999</v>
+      </c>
+      <c r="F8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>0.59328000000000003</v>
+      </c>
+      <c r="B9">
+        <v>0.18095</v>
+      </c>
+      <c r="C9">
+        <v>0.40860999999999997</v>
+      </c>
+      <c r="D9">
+        <v>0.57730000000000004</v>
+      </c>
+      <c r="E9">
+        <v>0.48866999999999999</v>
+      </c>
+      <c r="F9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>0.26308999999999999</v>
+      </c>
+      <c r="B10">
+        <v>0.35261999999999999</v>
+      </c>
+      <c r="C10">
+        <v>0.83752000000000004</v>
+      </c>
+      <c r="D10">
+        <v>0.81969999999999998</v>
+      </c>
+      <c r="E10">
+        <v>0.95169999999999999</v>
+      </c>
+      <c r="F10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>0.64576999999999996</v>
+      </c>
+      <c r="B11">
+        <v>0.56266000000000005</v>
+      </c>
+      <c r="C11">
+        <v>0.24948999999999999</v>
+      </c>
+      <c r="D11">
+        <v>0.67759000000000003</v>
+      </c>
+      <c r="E11">
+        <v>0.63100999999999996</v>
+      </c>
+      <c r="F11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>0.70430000000000004</v>
+      </c>
+      <c r="B12">
+        <v>0.68369000000000002</v>
+      </c>
+      <c r="C12">
+        <v>0.25791999999999998</v>
+      </c>
+      <c r="D12">
+        <v>0.45895999999999998</v>
+      </c>
+      <c r="E12">
+        <v>0.76912999999999998</v>
+      </c>
+      <c r="F12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>0.76644999999999996</v>
+      </c>
+      <c r="B13">
+        <v>0.72635000000000005</v>
+      </c>
+      <c r="C13">
+        <v>0.38603999999999999</v>
+      </c>
+      <c r="D13">
+        <v>0.64798999999999995</v>
+      </c>
+      <c r="E13">
+        <v>0.93440999999999996</v>
+      </c>
+      <c r="F13" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>0.85592000000000001</v>
+      </c>
+      <c r="B14">
+        <v>0.28633999999999998</v>
+      </c>
+      <c r="C14">
+        <v>2.852E-2</v>
+      </c>
+      <c r="D14">
+        <v>0.75033000000000005</v>
+      </c>
+      <c r="E14">
+        <v>0.16582</v>
+      </c>
+      <c r="F14" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>0.83616999999999997</v>
+      </c>
+      <c r="B15">
+        <v>0.23338</v>
+      </c>
+      <c r="C15">
+        <v>0.31281999999999999</v>
+      </c>
+      <c r="D15">
+        <v>0.37685999999999997</v>
+      </c>
+      <c r="E15">
+        <v>0.24265</v>
+      </c>
+      <c r="F15" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>0.41126000000000001</v>
+      </c>
+      <c r="B16">
+        <v>0.12496</v>
+      </c>
+      <c r="C16">
+        <v>0.26255000000000001</v>
+      </c>
+      <c r="D16">
+        <v>0.14774999999999999</v>
+      </c>
+      <c r="E16">
+        <v>0.33838000000000001</v>
+      </c>
+      <c r="F16" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>0.29435</v>
+      </c>
+      <c r="B17">
+        <v>0.33107999999999999</v>
+      </c>
+      <c r="C17">
+        <v>0.63988</v>
+      </c>
+      <c r="D17">
+        <v>0.52309000000000005</v>
+      </c>
+      <c r="E17">
+        <v>0.79898000000000002</v>
+      </c>
+      <c r="F17" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>0.15973000000000001</v>
+      </c>
+      <c r="B18">
+        <v>0.25816</v>
+      </c>
+      <c r="C18">
+        <v>9.5649999999999999E-2</v>
+      </c>
+      <c r="D18">
+        <v>0.25264999999999999</v>
+      </c>
+      <c r="E18">
+        <v>0.69567999999999997</v>
+      </c>
+      <c r="F18" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>0.96899999999999997</v>
+      </c>
+      <c r="B19">
+        <v>0.32417000000000001</v>
+      </c>
+      <c r="C19">
+        <v>0.33085999999999999</v>
+      </c>
+      <c r="D19">
+        <v>0.56032000000000004</v>
+      </c>
+      <c r="E19">
+        <v>0.18698999999999999</v>
+      </c>
+      <c r="F19" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>0.62411000000000005</v>
+      </c>
+      <c r="B20">
+        <v>0.82240000000000002</v>
+      </c>
+      <c r="C20">
+        <v>0.36007</v>
+      </c>
+      <c r="D20">
+        <v>0.89590000000000003</v>
+      </c>
+      <c r="E20">
+        <v>0.90139999999999998</v>
+      </c>
+      <c r="F20" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>0.63048999999999999</v>
+      </c>
+      <c r="B21">
+        <v>0.25719999999999998</v>
+      </c>
+      <c r="C21">
+        <v>0.39816000000000001</v>
+      </c>
+      <c r="D21">
+        <v>0.95126999999999995</v>
+      </c>
+      <c r="E21">
+        <v>0.23269000000000001</v>
+      </c>
+      <c r="F21" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>0.29586000000000001</v>
+      </c>
+      <c r="B22">
+        <v>0.56733999999999996</v>
+      </c>
+      <c r="C22">
+        <v>0.10943</v>
+      </c>
+      <c r="D22">
+        <v>7.0029999999999995E-2</v>
+      </c>
+      <c r="E22">
+        <v>0.89188000000000001</v>
+      </c>
+      <c r="F22" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>0.10659</v>
+      </c>
+      <c r="B23">
+        <v>0.29458000000000001</v>
+      </c>
+      <c r="C23">
+        <v>0.22020000000000001</v>
+      </c>
+      <c r="D23">
+        <v>0.74611000000000005</v>
+      </c>
+      <c r="E23">
+        <v>0.49695</v>
+      </c>
+      <c r="F23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>0.11703</v>
+      </c>
+      <c r="B24">
+        <v>0.29785</v>
+      </c>
+      <c r="C24">
+        <v>2.1010000000000001E-2</v>
+      </c>
+      <c r="D24">
+        <v>0.18756999999999999</v>
+      </c>
+      <c r="E24">
+        <v>0.38128000000000001</v>
+      </c>
+      <c r="F24" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>0.62348000000000003</v>
+      </c>
+      <c r="B25">
+        <v>0.63322000000000001</v>
+      </c>
+      <c r="C25">
+        <v>8.5419999999999996E-2</v>
+      </c>
+      <c r="D25">
+        <v>0.97141999999999995</v>
+      </c>
+      <c r="E25">
+        <v>0.29886000000000001</v>
+      </c>
+      <c r="F25" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>0.18276999999999999</v>
+      </c>
+      <c r="B26">
+        <v>0.37678</v>
+      </c>
+      <c r="C26">
+        <v>0.95482999999999996</v>
+      </c>
+      <c r="D26">
+        <v>0.55113000000000001</v>
+      </c>
+      <c r="E26">
+        <v>0.48133999999999999</v>
+      </c>
+      <c r="F26" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>1.511E-2</v>
+      </c>
+      <c r="B27">
+        <v>8.4959999999999994E-2</v>
+      </c>
+      <c r="C27">
+        <v>0.41032000000000002</v>
+      </c>
+      <c r="D27">
+        <v>0.54481999999999997</v>
+      </c>
+      <c r="E27">
+        <v>0.19541</v>
+      </c>
+      <c r="F27" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>0.12316000000000001</v>
+      </c>
+      <c r="B28">
+        <v>0.80308000000000002</v>
+      </c>
+      <c r="C28">
+        <v>0.68032999999999999</v>
+      </c>
+      <c r="D28">
+        <v>0.81537999999999999</v>
+      </c>
+      <c r="E28">
+        <v>0.96218999999999999</v>
+      </c>
+      <c r="F28" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>0.90246999999999999</v>
+      </c>
+      <c r="B29">
+        <v>0.97406999999999999</v>
+      </c>
+      <c r="C29">
+        <v>0.67351000000000005</v>
+      </c>
+      <c r="D29">
+        <v>0.51805000000000001</v>
+      </c>
+      <c r="E29">
+        <v>0.35376000000000002</v>
+      </c>
+      <c r="F29" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>0.83950999999999998</v>
+      </c>
+      <c r="B30">
+        <v>0.65042</v>
+      </c>
+      <c r="C30">
+        <v>0.62044999999999995</v>
+      </c>
+      <c r="D30">
+        <v>5.5590000000000001E-2</v>
+      </c>
+      <c r="E30">
+        <v>0.13378999999999999</v>
+      </c>
+      <c r="F30" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>0.95433999999999997</v>
+      </c>
+      <c r="B31">
+        <v>0.89871000000000001</v>
+      </c>
+      <c r="C31">
+        <v>0.57576000000000005</v>
+      </c>
+      <c r="D31">
+        <v>0.52952999999999995</v>
+      </c>
+      <c r="E31">
+        <v>0.19994999999999999</v>
+      </c>
+      <c r="F31" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>0.84065999999999996</v>
+      </c>
+      <c r="B32">
+        <v>0.96686000000000005</v>
+      </c>
+      <c r="C32">
+        <v>0.54503999999999997</v>
+      </c>
+      <c r="D32">
+        <v>0.59921000000000002</v>
+      </c>
+      <c r="E32">
+        <v>0.47493000000000002</v>
+      </c>
+      <c r="F32" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>0.75866999999999996</v>
+      </c>
+      <c r="B33">
+        <v>0.70515000000000005</v>
+      </c>
+      <c r="C33">
+        <v>0.34068999999999999</v>
+      </c>
+      <c r="D33">
+        <v>0.21765999999999999</v>
+      </c>
+      <c r="E33">
+        <v>0.20144000000000001</v>
+      </c>
+      <c r="F33" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>0.50343000000000004</v>
+      </c>
+      <c r="B34">
+        <v>0.80730000000000002</v>
+      </c>
+      <c r="C34">
+        <v>0.38423000000000002</v>
+      </c>
+      <c r="D34">
+        <v>6.3640000000000002E-2</v>
+      </c>
+      <c r="E34">
+        <v>2.7230000000000001E-2</v>
+      </c>
+      <c r="F34" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>0.12681000000000001</v>
+      </c>
+      <c r="B35">
+        <v>0.15423999999999999</v>
+      </c>
+      <c r="C35">
+        <v>0.48000999999999999</v>
+      </c>
+      <c r="D35">
+        <v>0.96887999999999996</v>
+      </c>
+      <c r="E35">
+        <v>0.73575999999999997</v>
+      </c>
+      <c r="F35" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>0.40616000000000002</v>
+      </c>
+      <c r="B36">
+        <v>0.15426999999999999</v>
+      </c>
+      <c r="C36">
+        <v>0.39380999999999999</v>
+      </c>
+      <c r="D36">
+        <v>0.87121999999999999</v>
+      </c>
+      <c r="E36">
+        <v>0.75168999999999997</v>
+      </c>
+      <c r="F36" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>0.95926</v>
+      </c>
+      <c r="B37">
+        <v>0.92510000000000003</v>
+      </c>
+      <c r="C37">
+        <v>0.63539000000000001</v>
+      </c>
+      <c r="D37">
+        <v>0.66125</v>
+      </c>
+      <c r="E37">
+        <v>0.72338999999999998</v>
+      </c>
+      <c r="F37" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>0.4516</v>
+      </c>
+      <c r="B38">
+        <v>0.78993000000000002</v>
+      </c>
+      <c r="C38">
+        <v>0.91500999999999999</v>
+      </c>
+      <c r="D38">
+        <v>0.97224999999999995</v>
+      </c>
+      <c r="E38">
+        <v>0.72960999999999998</v>
+      </c>
+      <c r="F38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>0.66302000000000005</v>
+      </c>
+      <c r="B39">
+        <v>0.92793999999999999</v>
+      </c>
+      <c r="C39">
+        <v>0.35694999999999999</v>
+      </c>
+      <c r="D39">
+        <v>0.84011000000000002</v>
+      </c>
+      <c r="E39">
+        <v>2.2700000000000001E-2</v>
+      </c>
+      <c r="F39" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>0.66957</v>
+      </c>
+      <c r="B40">
+        <v>0.99878</v>
+      </c>
+      <c r="C40">
+        <v>0.87070999999999998</v>
+      </c>
+      <c r="D40">
+        <v>0.42320000000000002</v>
+      </c>
+      <c r="E40">
+        <v>0.39921000000000001</v>
+      </c>
+      <c r="F40" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>0.97494999999999998</v>
+      </c>
+      <c r="B41">
+        <v>0.19411</v>
+      </c>
+      <c r="C41">
+        <v>0.98031999999999997</v>
+      </c>
+      <c r="D41">
+        <v>0.19728999999999999</v>
+      </c>
+      <c r="E41">
+        <v>0.27986</v>
+      </c>
+      <c r="F41" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>0.67642000000000002</v>
+      </c>
+      <c r="B42">
+        <v>0.81101000000000001</v>
+      </c>
+      <c r="C42">
+        <v>0.25903999999999999</v>
+      </c>
+      <c r="D42">
+        <v>3.3300000000000003E-2</v>
+      </c>
+      <c r="E42">
+        <v>0.44753999999999999</v>
+      </c>
+      <c r="F42" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>0.21340000000000001</v>
+      </c>
+      <c r="B43">
+        <v>0.68176999999999999</v>
+      </c>
+      <c r="C43">
+        <v>0.80759000000000003</v>
+      </c>
+      <c r="D43">
+        <v>0.48409999999999997</v>
+      </c>
+      <c r="E43">
+        <v>0.93962999999999997</v>
+      </c>
+      <c r="F43" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>7.1050000000000002E-2</v>
+      </c>
+      <c r="B44">
+        <v>0.75249999999999995</v>
+      </c>
+      <c r="C44">
+        <v>0.70550999999999997</v>
+      </c>
+      <c r="D44">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="E44">
+        <v>0.5958</v>
+      </c>
+      <c r="F44" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>3.5720000000000002E-2</v>
+      </c>
+      <c r="B45">
+        <v>5.3039999999999997E-2</v>
+      </c>
+      <c r="C45">
+        <v>0.70274999999999999</v>
+      </c>
+      <c r="D45">
+        <v>0.29987000000000003</v>
+      </c>
+      <c r="E45">
+        <v>0.72479000000000005</v>
+      </c>
+      <c r="F45" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>0.94635000000000002</v>
+      </c>
+      <c r="B46">
+        <v>0.31974999999999998</v>
+      </c>
+      <c r="C46">
+        <v>0.90190999999999999</v>
+      </c>
+      <c r="D46">
+        <v>0.35969000000000001</v>
+      </c>
+      <c r="E46">
+        <v>0.85924999999999996</v>
+      </c>
+      <c r="F46" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>0.4002</v>
+      </c>
+      <c r="B47">
+        <v>0.80361000000000005</v>
+      </c>
+      <c r="C47">
+        <v>0.53142</v>
+      </c>
+      <c r="D47">
+        <v>1.221E-2</v>
+      </c>
+      <c r="E47">
+        <v>0.14052999999999999</v>
+      </c>
+      <c r="F47" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>0.51190000000000002</v>
+      </c>
+      <c r="B48">
+        <v>0.20166000000000001</v>
+      </c>
+      <c r="C48">
+        <v>0.81364000000000003</v>
+      </c>
+      <c r="D48">
+        <v>0.45590999999999998</v>
+      </c>
+      <c r="E48">
+        <v>0.68608000000000002</v>
+      </c>
+      <c r="F48" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>0.98756999999999995</v>
+      </c>
+      <c r="B49">
+        <v>0.54083000000000003</v>
+      </c>
+      <c r="C49">
+        <v>4.5999999999999999E-3</v>
+      </c>
+      <c r="D49">
+        <v>1.9699999999999999E-2</v>
+      </c>
+      <c r="E49">
+        <v>0.46561999999999998</v>
+      </c>
+      <c r="F49" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>0.52978999999999998</v>
+      </c>
+      <c r="B50">
+        <v>0.76593999999999995</v>
+      </c>
+      <c r="C50">
+        <v>0.8155</v>
+      </c>
+      <c r="D50">
+        <v>0.12058000000000001</v>
+      </c>
+      <c r="E50">
+        <v>0.33964</v>
+      </c>
+      <c r="F50" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>5.4199999999999998E-2</v>
+      </c>
+      <c r="B51">
+        <v>0.95306000000000002</v>
+      </c>
+      <c r="C51">
+        <v>0.20668</v>
+      </c>
+      <c r="D51">
+        <v>0.27984999999999999</v>
+      </c>
+      <c r="E51">
+        <v>0.67998000000000003</v>
+      </c>
+      <c r="F51" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>0.55930000000000002</v>
+      </c>
+      <c r="B52">
+        <v>0.39859</v>
+      </c>
+      <c r="C52">
+        <v>0.96853999999999996</v>
+      </c>
+      <c r="D52">
+        <v>0.17682999999999999</v>
+      </c>
+      <c r="E52">
+        <v>0.72813000000000005</v>
+      </c>
+      <c r="F52" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>0.14949999999999999</v>
+      </c>
+      <c r="B53">
+        <v>0.77814000000000005</v>
+      </c>
+      <c r="C53">
+        <v>0.54246000000000005</v>
+      </c>
+      <c r="D53">
+        <v>0.82171000000000005</v>
+      </c>
+      <c r="E53">
+        <v>0.17671000000000001</v>
+      </c>
+      <c r="F53" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>0.36646000000000001</v>
+      </c>
+      <c r="B54">
+        <v>0.81815000000000004</v>
+      </c>
+      <c r="C54">
+        <v>0.87361999999999995</v>
+      </c>
+      <c r="D54">
+        <v>0.72768999999999995</v>
+      </c>
+      <c r="E54">
+        <v>0.22276000000000001</v>
+      </c>
+      <c r="F54" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>0.56916999999999995</v>
+      </c>
+      <c r="B55">
+        <v>0.17019999999999999</v>
+      </c>
+      <c r="C55">
+        <v>0.60270999999999997</v>
+      </c>
+      <c r="D55">
+        <v>0.68576999999999999</v>
+      </c>
+      <c r="E55">
+        <v>0.15211</v>
+      </c>
+      <c r="F55" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>0.80393000000000003</v>
+      </c>
+      <c r="B56">
+        <v>7.3270000000000002E-2</v>
+      </c>
+      <c r="C56">
+        <v>0.70601000000000003</v>
+      </c>
+      <c r="D56">
+        <v>0.44742999999999999</v>
+      </c>
+      <c r="E56">
+        <v>0.29881999999999997</v>
+      </c>
+      <c r="F56" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>0.26761000000000001</v>
+      </c>
+      <c r="B57">
+        <v>0.15669</v>
+      </c>
+      <c r="C57">
+        <v>0.85431000000000001</v>
+      </c>
+      <c r="D57">
+        <v>0.51553000000000004</v>
+      </c>
+      <c r="E57">
+        <v>0.22015000000000001</v>
+      </c>
+      <c r="F57" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>0.23755999999999999</v>
+      </c>
+      <c r="B58">
+        <v>0.65717999999999999</v>
+      </c>
+      <c r="C58">
+        <v>0.38246999999999998</v>
+      </c>
+      <c r="D58">
+        <v>0.34182000000000001</v>
+      </c>
+      <c r="E58">
+        <v>0.58813000000000004</v>
+      </c>
+      <c r="F58" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>0.25792999999999999</v>
+      </c>
+      <c r="B59">
+        <v>3.49E-2</v>
+      </c>
+      <c r="C59">
+        <v>0.93574999999999997</v>
+      </c>
+      <c r="D59">
+        <v>0.95979999999999999</v>
+      </c>
+      <c r="E59">
+        <v>0.39566000000000001</v>
+      </c>
+      <c r="F59" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>4.5100000000000001E-2</v>
+      </c>
+      <c r="B60">
+        <v>0.95857999999999999</v>
+      </c>
+      <c r="C60">
+        <v>0.47298000000000001</v>
+      </c>
+      <c r="D60">
+        <v>0.85563</v>
+      </c>
+      <c r="E60">
+        <v>0.71382000000000001</v>
+      </c>
+      <c r="F60" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>5.2139999999999999E-2</v>
+      </c>
+      <c r="B61">
+        <v>0.79044999999999999</v>
+      </c>
+      <c r="C61">
+        <v>0.89525999999999994</v>
+      </c>
+      <c r="D61">
+        <v>0.40858</v>
+      </c>
+      <c r="E61">
+        <v>0.60492999999999997</v>
+      </c>
+      <c r="F61" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>0.70804</v>
+      </c>
+      <c r="B62">
+        <v>0.25475999999999999</v>
+      </c>
+      <c r="C62">
+        <v>0.80874999999999997</v>
+      </c>
+      <c r="D62">
+        <v>0.99187000000000003</v>
+      </c>
+      <c r="E62">
+        <v>0.43918000000000001</v>
+      </c>
+      <c r="F62" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>0.15869</v>
+      </c>
+      <c r="B63">
+        <v>0.76853000000000005</v>
+      </c>
+      <c r="C63">
+        <v>0.44206000000000001</v>
+      </c>
+      <c r="D63">
+        <v>0.69662000000000002</v>
+      </c>
+      <c r="E63">
+        <v>0.74853000000000003</v>
+      </c>
+      <c r="F63" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>4.453E-2</v>
+      </c>
+      <c r="B64">
+        <v>0.52690999999999999</v>
+      </c>
+      <c r="C64">
+        <v>0.78580000000000005</v>
+      </c>
+      <c r="D64">
+        <v>0.55518999999999996</v>
+      </c>
+      <c r="E64">
+        <v>0.71226</v>
+      </c>
+      <c r="F64" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>0.30743999999999999</v>
+      </c>
+      <c r="B65">
+        <v>0.56659000000000004</v>
+      </c>
+      <c r="C65">
+        <v>0.90595000000000003</v>
+      </c>
+      <c r="D65">
+        <v>0.13797999999999999</v>
+      </c>
+      <c r="E65">
+        <v>0.42115000000000002</v>
+      </c>
+      <c r="F65" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>0.63039999999999996</v>
+      </c>
+      <c r="B66">
+        <v>0.30197000000000002</v>
+      </c>
+      <c r="C66">
+        <v>0.95594000000000001</v>
+      </c>
+      <c r="D66">
+        <v>0.41088000000000002</v>
+      </c>
+      <c r="E66">
+        <v>0.14990999999999999</v>
+      </c>
+      <c r="F66" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>0.95987999999999996</v>
+      </c>
+      <c r="B67">
+        <v>0.15784000000000001</v>
+      </c>
+      <c r="C67">
+        <v>0.83616999999999997</v>
+      </c>
+      <c r="D67">
+        <v>0.12637999999999999</v>
+      </c>
+      <c r="E67">
+        <v>0.73802999999999996</v>
+      </c>
+      <c r="F67" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>0.75239</v>
+      </c>
+      <c r="B68">
+        <v>0.3836</v>
+      </c>
+      <c r="C68">
+        <v>0.80408999999999997</v>
+      </c>
+      <c r="D68">
+        <v>0.97960999999999998</v>
+      </c>
+      <c r="E68">
+        <v>0.12285</v>
+      </c>
+      <c r="F68" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>0.93737999999999999</v>
+      </c>
+      <c r="B69">
+        <v>0.76251999999999998</v>
+      </c>
+      <c r="C69">
+        <v>0.11044</v>
+      </c>
+      <c r="D69">
+        <v>0.26332</v>
+      </c>
+      <c r="E69">
+        <v>0.17247000000000001</v>
+      </c>
+      <c r="F69" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A1:F69">
+    <sortCondition ref="F1:F69"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>